<commit_message>
Fix regression models and applying minor changes to the code
</commit_message>
<xml_diff>
--- a/Jupyter/Python/resultados_distribuicoes.xlsx
+++ b/Jupyter/Python/resultados_distribuicoes.xlsx
@@ -488,7 +488,7 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.964035964035964</v>
+        <v>0.974025974025974</v>
       </c>
     </row>
     <row r="3">
@@ -514,7 +514,7 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>0.3686313686313686</v>
+        <v>0.3706293706293706</v>
       </c>
     </row>
     <row r="4">
@@ -540,7 +540,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>0.6783216783216783</v>
+        <v>0.7022977022977023</v>
       </c>
     </row>
     <row r="5">
@@ -566,7 +566,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>0.2097902097902098</v>
+        <v>0.2427572427572428</v>
       </c>
     </row>
     <row r="6">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>0.01998001998001998</v>
+        <v>0.01698301698301698</v>
       </c>
     </row>
     <row r="7">
@@ -1008,7 +1008,7 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>0.7932067932067932</v>
+        <v>0.8071928071928072</v>
       </c>
     </row>
     <row r="23">
@@ -1034,7 +1034,7 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>0.2247752247752248</v>
+        <v>0.2177822177822178</v>
       </c>
     </row>
     <row r="24">
@@ -1060,7 +1060,7 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>0.5764235764235764</v>
+        <v>0.6183816183816184</v>
       </c>
     </row>
     <row r="25">
@@ -1086,7 +1086,7 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>0.6913086913086913</v>
+        <v>0.6803196803196803</v>
       </c>
     </row>
     <row r="26">
@@ -1112,7 +1112,7 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>0.04995004995004995</v>
+        <v>0.04795204795204795</v>
       </c>
     </row>
     <row r="27">
@@ -1372,7 +1372,7 @@
         </is>
       </c>
       <c r="F36" t="n">
-        <v>0.06913916129627529</v>
+        <v>0.06913916129627551</v>
       </c>
     </row>
     <row r="37">
@@ -1554,7 +1554,7 @@
         </is>
       </c>
       <c r="F43" t="n">
-        <v>0.005994005994005994</v>
+        <v>0.008991008991008992</v>
       </c>
     </row>
     <row r="44">
@@ -1580,7 +1580,7 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>0.8661338661338661</v>
+        <v>0.8551448551448552</v>
       </c>
     </row>
     <row r="45">
@@ -1788,7 +1788,7 @@
         </is>
       </c>
       <c r="F52" t="n">
-        <v>2.469022573536872e-05</v>
+        <v>2.469022573559077e-05</v>
       </c>
     </row>
     <row r="53">
@@ -2048,7 +2048,7 @@
         </is>
       </c>
       <c r="F62" t="n">
-        <v>0.6693306693306693</v>
+        <v>0.6883116883116883</v>
       </c>
     </row>
     <row r="63">
@@ -2074,7 +2074,7 @@
         </is>
       </c>
       <c r="F63" t="n">
-        <v>0.2727272727272727</v>
+        <v>0.2407592407592408</v>
       </c>
     </row>
     <row r="64">
@@ -2100,7 +2100,7 @@
         </is>
       </c>
       <c r="F64" t="n">
-        <v>0.5614385614385614</v>
+        <v>0.5664335664335665</v>
       </c>
     </row>
     <row r="65">
@@ -2152,7 +2152,7 @@
         </is>
       </c>
       <c r="F66" t="n">
-        <v>0.2757242757242757</v>
+        <v>0.2727272727272727</v>
       </c>
     </row>
     <row r="67">
@@ -2620,7 +2620,7 @@
         </is>
       </c>
       <c r="F84" t="n">
-        <v>0.06393606393606394</v>
+        <v>0.08291708291708291</v>
       </c>
     </row>
     <row r="85">
@@ -2828,7 +2828,7 @@
         </is>
       </c>
       <c r="F92" t="n">
-        <v>9.436353815006626e-07</v>
+        <v>9.436353817227072e-07</v>
       </c>
     </row>
     <row r="93">
@@ -2880,7 +2880,7 @@
         </is>
       </c>
       <c r="F94" t="n">
-        <v>0.3112203730524644</v>
+        <v>0.3112203730524643</v>
       </c>
     </row>
     <row r="95">
@@ -3088,7 +3088,7 @@
         </is>
       </c>
       <c r="F102" t="n">
-        <v>0.4125874125874126</v>
+        <v>0.4305694305694306</v>
       </c>
     </row>
     <row r="103">
@@ -3114,7 +3114,7 @@
         </is>
       </c>
       <c r="F103" t="n">
-        <v>0.4775224775224775</v>
+        <v>0.4415584415584415</v>
       </c>
     </row>
     <row r="104">
@@ -3140,7 +3140,7 @@
         </is>
       </c>
       <c r="F104" t="n">
-        <v>0.3726273726273726</v>
+        <v>0.3766233766233766</v>
       </c>
     </row>
     <row r="105">
@@ -3166,7 +3166,7 @@
         </is>
       </c>
       <c r="F105" t="n">
-        <v>0.2577422577422577</v>
+        <v>0.2457542457542458</v>
       </c>
     </row>
     <row r="106">
@@ -3192,7 +3192,7 @@
         </is>
       </c>
       <c r="F106" t="n">
-        <v>0.3576423576423576</v>
+        <v>0.3476523476523476</v>
       </c>
     </row>
     <row r="107">
@@ -3608,7 +3608,7 @@
         </is>
       </c>
       <c r="F122" t="n">
-        <v>0.01898101898101898</v>
+        <v>0.02997002997002997</v>
       </c>
     </row>
     <row r="123">
@@ -3634,7 +3634,7 @@
         </is>
       </c>
       <c r="F123" t="n">
-        <v>0.2317682317682318</v>
+        <v>0.2167832167832168</v>
       </c>
     </row>
     <row r="124">
@@ -3660,7 +3660,7 @@
         </is>
       </c>
       <c r="F124" t="n">
-        <v>0.3676323676323676</v>
+        <v>0.3756243756243756</v>
       </c>
     </row>
     <row r="125">
@@ -3686,7 +3686,7 @@
         </is>
       </c>
       <c r="F125" t="n">
-        <v>0.008991008991008992</v>
+        <v>0.006993006993006993</v>
       </c>
     </row>
     <row r="126">
@@ -3712,7 +3712,7 @@
         </is>
       </c>
       <c r="F126" t="n">
-        <v>0.02097902097902098</v>
+        <v>0.01698301698301698</v>
       </c>
     </row>
     <row r="127">
@@ -3868,7 +3868,7 @@
         </is>
       </c>
       <c r="F132" t="n">
-        <v>0.004523816040784667</v>
+        <v>0.004523816040785111</v>
       </c>
     </row>
     <row r="133">
@@ -3894,7 +3894,7 @@
         </is>
       </c>
       <c r="F133" t="n">
-        <v>0.1498957763688196</v>
+        <v>0.1498957763688197</v>
       </c>
     </row>
     <row r="134">
@@ -3972,7 +3972,7 @@
         </is>
       </c>
       <c r="F136" t="n">
-        <v>0.02328618390033743</v>
+        <v>0.02328618390033799</v>
       </c>
     </row>
     <row r="137">
@@ -4128,7 +4128,7 @@
         </is>
       </c>
       <c r="F142" t="n">
-        <v>0.06393606393606394</v>
+        <v>0.05994005994005994</v>
       </c>
     </row>
     <row r="143">
@@ -4154,7 +4154,7 @@
         </is>
       </c>
       <c r="F143" t="n">
-        <v>0.02697302697302697</v>
+        <v>0.03196803196803197</v>
       </c>
     </row>
     <row r="144">
@@ -4180,7 +4180,7 @@
         </is>
       </c>
       <c r="F144" t="n">
-        <v>0.3336663336663337</v>
+        <v>0.3086913086913087</v>
       </c>
     </row>
     <row r="145">
@@ -4206,7 +4206,7 @@
         </is>
       </c>
       <c r="F145" t="n">
-        <v>0.01198801198801199</v>
+        <v>0.01598401598401598</v>
       </c>
     </row>
     <row r="146">
@@ -4232,7 +4232,7 @@
         </is>
       </c>
       <c r="F146" t="n">
-        <v>0.06893106893106893</v>
+        <v>0.07292707292707293</v>
       </c>
     </row>
     <row r="147">
@@ -4414,7 +4414,7 @@
         </is>
       </c>
       <c r="F153" t="n">
-        <v>0.02332817845416735</v>
+        <v>0.0233281784541669</v>
       </c>
     </row>
     <row r="154">
@@ -4648,7 +4648,7 @@
         </is>
       </c>
       <c r="F162" t="n">
-        <v>0.04795204795204795</v>
+        <v>0.05794205794205794</v>
       </c>
     </row>
     <row r="163">
@@ -4674,7 +4674,7 @@
         </is>
       </c>
       <c r="F163" t="n">
-        <v>0.02397602397602398</v>
+        <v>0.03296703296703297</v>
       </c>
     </row>
     <row r="164">
@@ -4700,7 +4700,7 @@
         </is>
       </c>
       <c r="F164" t="n">
-        <v>0.01898101898101898</v>
+        <v>0.02097902097902098</v>
       </c>
     </row>
     <row r="165">
@@ -4726,7 +4726,7 @@
         </is>
       </c>
       <c r="F165" t="n">
-        <v>0.1088911088911089</v>
+        <v>0.08691308691308691</v>
       </c>
     </row>
     <row r="166">
@@ -4752,7 +4752,7 @@
         </is>
       </c>
       <c r="F166" t="n">
-        <v>0.05094905094905095</v>
+        <v>0.05194805194805195</v>
       </c>
     </row>
     <row r="167">
@@ -4934,7 +4934,7 @@
         </is>
       </c>
       <c r="F173" t="n">
-        <v>0.08041604217813514</v>
+        <v>0.08041604217813469</v>
       </c>
     </row>
     <row r="174">
@@ -5194,7 +5194,7 @@
         </is>
       </c>
       <c r="F183" t="n">
-        <v>0.00999000999000999</v>
+        <v>0.01298701298701299</v>
       </c>
     </row>
     <row r="184">
@@ -5220,7 +5220,7 @@
         </is>
       </c>
       <c r="F184" t="n">
-        <v>0.01998001998001998</v>
+        <v>0.01798201798201798</v>
       </c>
     </row>
     <row r="185">
@@ -5246,7 +5246,7 @@
         </is>
       </c>
       <c r="F185" t="n">
-        <v>0.1228771228771229</v>
+        <v>0.1028971028971029</v>
       </c>
     </row>
     <row r="186">
@@ -5272,7 +5272,7 @@
         </is>
       </c>
       <c r="F186" t="n">
-        <v>0.1628371628371628</v>
+        <v>0.1708291708291708</v>
       </c>
     </row>
     <row r="187">
@@ -5454,7 +5454,7 @@
         </is>
       </c>
       <c r="F193" t="n">
-        <v>0.07037774599087132</v>
+        <v>0.0703777459908711</v>
       </c>
     </row>
     <row r="194">

</xml_diff>